<commit_message>
updating app to read data from excel file instead of fetching the api everytime
</commit_message>
<xml_diff>
--- a/NVDA_stock_data.xlsx
+++ b/NVDA_stock_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,1171 +471,2461 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45443</v>
+        <v>45502</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1125.2000</t>
+          <t>113.6900</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1127.1700</t>
+          <t>116.2800</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1069.4000</t>
+          <t>111.3000</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1096.3300</t>
+          <t>111.5900</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>61326250</t>
+          <t>248152068</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45446</v>
+        <v>45499</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1136.2100</t>
+          <t>116.1900</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1150.0000</t>
+          <t>116.2000</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1120.0300</t>
+          <t>111.5800</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1150.0000</t>
+          <t>113.0600</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>43839176</t>
+          <t>293399073</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45447</v>
+        <v>45498</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1157.1600</t>
+          <t>113.0400</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1166.0000</t>
+          <t>116.6300</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1140.4500</t>
+          <t>106.3000</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1164.3700</t>
+          <t>112.2800</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>40332401</t>
+          <t>460067019</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45448</v>
+        <v>45497</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1183.7100</t>
+          <t>119.1700</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1224.4950</t>
+          <t>119.9500</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1174.6800</t>
+          <t>113.4400</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1224.4000</t>
+          <t>114.2500</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>52840178</t>
+          <t>327776884</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45449</v>
+        <v>45496</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1240.4800</t>
+          <t>122.7800</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1255.8700</t>
+          <t>124.6900</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1183.2000</t>
+          <t>122.1000</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1209.9800</t>
+          <t>122.5900</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>66469619</t>
+          <t>173910983</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45450</v>
+        <v>45495</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1197.7000</t>
+          <t>120.3500</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1216.9171</t>
+          <t>124.0700</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1180.2200</t>
+          <t>119.8600</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1208.8800</t>
+          <t>123.5400</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>41238580</t>
+          <t>258068943</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45453</v>
+        <v>45492</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>120.3700</t>
+          <t>120.3500</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>123.1000</t>
+          <t>121.6000</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>117.0100</t>
+          <t>117.3700</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>121.7900</t>
+          <t>117.9300</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>308134791</t>
+          <t>217223800</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45454</v>
+        <v>45491</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>121.7700</t>
+          <t>121.8500</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>122.8700</t>
+          <t>122.4000</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>118.7400</t>
+          <t>116.5600</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>120.9100</t>
+          <t>121.0900</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>222551158</t>
+          <t>320979530</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45455</v>
+        <v>45490</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>123.0600</t>
+          <t>121.3500</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>126.8800</t>
+          <t>121.8500</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>122.5700</t>
+          <t>116.7200</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>125.2000</t>
+          <t>117.9900</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>299595001</t>
+          <t>390086189</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45456</v>
+        <v>45489</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>129.3900</t>
+          <t>128.4400</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>129.8000</t>
+          <t>129.0400</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>127.1600</t>
+          <t>124.5800</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>129.6100</t>
+          <t>126.3600</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>260704537</t>
+          <t>214769515</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45457</v>
+        <v>45488</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>129.9600</t>
+          <t>130.5600</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>132.8400</t>
+          <t>131.3900</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>128.3200</t>
+          <t>127.1800</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>131.8800</t>
+          <t>128.4400</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>309320376</t>
+          <t>208326164</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45460</v>
+        <v>45485</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>132.9900</t>
+          <t>128.2600</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>133.7300</t>
+          <t>131.9200</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>129.5800</t>
+          <t>127.2200</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>130.9800</t>
+          <t>129.2400</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>288504444</t>
+          <t>252680535</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45461</v>
+        <v>45484</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>131.1400</t>
+          <t>135.7500</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>136.3300</t>
+          <t>136.1500</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>130.6900</t>
+          <t>127.0500</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>135.5800</t>
+          <t>127.4000</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>294335054</t>
+          <t>374782738</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45463</v>
+        <v>45483</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>139.8000</t>
+          <t>134.0300</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>140.7600</t>
+          <t>135.1000</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>129.5200</t>
+          <t>132.4200</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>130.7800</t>
+          <t>134.9100</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>517768425</t>
+          <t>248978569</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45464</v>
+        <v>45482</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>127.1200</t>
+          <t>130.3500</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>130.6300</t>
+          <t>133.8200</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>124.3000</t>
+          <t>128.6500</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>126.5700</t>
+          <t>131.3800</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>655484664</t>
+          <t>287020820</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45467</v>
+        <v>45481</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>123.2400</t>
+          <t>127.4900</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>124.4600</t>
+          <t>130.7700</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>118.0400</t>
+          <t>127.0400</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>118.1100</t>
+          <t>128.2000</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>476060866</t>
+          <t>237677322</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45468</v>
+        <v>45478</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>121.2000</t>
+          <t>127.3800</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>126.5000</t>
+          <t>128.8500</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>119.3200</t>
+          <t>125.6800</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>126.0900</t>
+          <t>125.8300</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>425787456</t>
+          <t>214176689</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45469</v>
+        <v>45476</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>126.1300</t>
+          <t>121.6600</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>128.1200</t>
+          <t>128.2800</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>122.6000</t>
+          <t>121.3600</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>126.4000</t>
+          <t>128.2800</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>362975918</t>
+          <t>215748955</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45470</v>
+        <v>45475</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>124.1000</t>
+          <t>121.1300</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>126.4100</t>
+          <t>123.4100</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>122.9200</t>
+          <t>121.0300</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>123.9900</t>
+          <t>122.6700</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>252571693</t>
+          <t>218373969</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45471</v>
+        <v>45474</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>124.5800</t>
+          <t>123.4700</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>127.7100</t>
+          <t>124.8400</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>122.7500</t>
+          <t>118.8300</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>123.5400</t>
+          <t>124.3000</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>315516740</t>
+          <t>284885534</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45474</v>
+        <v>45471</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>123.4700</t>
+          <t>124.5800</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>124.8400</t>
+          <t>127.7100</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>118.8300</t>
+          <t>122.7500</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>124.3000</t>
+          <t>123.5400</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>284885534</t>
+          <t>315516740</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45475</v>
+        <v>45470</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>121.1300</t>
+          <t>124.1000</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>123.4100</t>
+          <t>126.4100</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>121.0300</t>
+          <t>122.9200</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>122.6700</t>
+          <t>123.9900</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>218373969</t>
+          <t>252571693</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45476</v>
+        <v>45469</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>121.6600</t>
+          <t>126.1300</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>128.2800</t>
+          <t>128.1200</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>121.3600</t>
+          <t>122.6000</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>128.2800</t>
+          <t>126.4000</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>215748955</t>
+          <t>362975918</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45478</v>
+        <v>45468</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>127.3800</t>
+          <t>121.2000</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>128.8500</t>
+          <t>126.5000</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>125.6800</t>
+          <t>119.3200</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>125.8300</t>
+          <t>126.0900</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>214176689</t>
+          <t>425787456</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45481</v>
+        <v>45467</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>127.4900</t>
+          <t>123.2400</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>130.7700</t>
+          <t>124.4600</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>127.0400</t>
+          <t>118.0400</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>128.2000</t>
+          <t>118.1100</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>237677322</t>
+          <t>476060866</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45482</v>
+        <v>45464</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>130.3500</t>
+          <t>127.1200</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>133.8200</t>
+          <t>130.6300</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>128.6500</t>
+          <t>124.3000</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>131.3800</t>
+          <t>126.5700</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>287020820</t>
+          <t>655484664</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45483</v>
+        <v>45463</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>134.0300</t>
+          <t>139.8000</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>135.1000</t>
+          <t>140.7600</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>132.4200</t>
+          <t>129.5200</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>134.9100</t>
+          <t>130.7800</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>248978569</t>
+          <t>517768425</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45484</v>
+        <v>45461</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>135.7500</t>
+          <t>131.1400</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>136.1500</t>
+          <t>136.3300</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>127.0500</t>
+          <t>130.6900</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>127.4000</t>
+          <t>135.5800</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>374782738</t>
+          <t>294335054</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45485</v>
+        <v>45460</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>128.2600</t>
+          <t>132.9900</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>131.9200</t>
+          <t>133.7300</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>127.2200</t>
+          <t>129.5800</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>129.2400</t>
+          <t>130.9800</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>252680535</t>
+          <t>288504444</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45488</v>
+        <v>45457</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>130.5600</t>
+          <t>129.9600</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>131.3900</t>
+          <t>132.8400</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>127.1800</t>
+          <t>128.3200</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>128.4400</t>
+          <t>131.8800</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>208326164</t>
+          <t>309320376</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45489</v>
+        <v>45456</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>128.4400</t>
+          <t>129.3900</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>129.0400</t>
+          <t>129.8000</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>124.5800</t>
+          <t>127.1600</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>126.3600</t>
+          <t>129.6100</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>214769515</t>
+          <t>260704537</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45490</v>
+        <v>45455</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>121.3500</t>
+          <t>123.0600</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>121.8500</t>
+          <t>126.8800</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>116.7200</t>
+          <t>122.5700</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>117.9900</t>
+          <t>125.2000</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>390086189</t>
+          <t>299595001</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45491</v>
+        <v>45454</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>121.8500</t>
+          <t>121.7700</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>122.4000</t>
+          <t>122.8700</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>116.5600</t>
+          <t>118.7400</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>121.0900</t>
+          <t>120.9100</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>320979530</t>
+          <t>222551158</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45492</v>
+        <v>45453</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>120.3500</t>
+          <t>120.3700</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>121.6000</t>
+          <t>123.1000</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>117.3700</t>
+          <t>117.0100</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>117.9300</t>
+          <t>121.7900</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>217223800</t>
+          <t>308134791</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45495</v>
+        <v>45450</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>120.3500</t>
+          <t>1197.7000</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>124.0700</t>
+          <t>1216.9171</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>119.8600</t>
+          <t>1180.2200</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>123.5400</t>
+          <t>1208.8800</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>258068943</t>
+          <t>41238580</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45496</v>
+        <v>45449</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>122.7800</t>
+          <t>1240.4800</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>124.6900</t>
+          <t>1255.8700</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>122.1000</t>
+          <t>1183.2000</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>122.5900</t>
+          <t>1209.9800</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>173910983</t>
+          <t>66469619</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45497</v>
+        <v>45448</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>119.1700</t>
+          <t>1183.7100</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>119.9500</t>
+          <t>1224.4950</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>113.4400</t>
+          <t>1174.6800</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>114.2500</t>
+          <t>1224.4000</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>327776884</t>
+          <t>52840178</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45498</v>
+        <v>45447</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>113.0400</t>
+          <t>1157.1600</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>116.6300</t>
+          <t>1166.0000</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>106.3000</t>
+          <t>1140.4500</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>112.2800</t>
+          <t>1164.3700</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>460067019</t>
+          <t>40332401</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45499</v>
+        <v>45446</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>116.1900</t>
+          <t>1136.2100</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>116.2000</t>
+          <t>1150.0000</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>111.5800</t>
+          <t>1120.0300</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>113.0600</t>
+          <t>1150.0000</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>293399073</t>
+          <t>43839176</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>45443</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>1125.2000</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>1127.1700</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>1069.4000</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>1096.3300</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>61326250</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45442</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>1146.5000</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>1158.1915</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>1096.6300</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>1105.0000</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>48735033</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>1130.5000</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>1154.9200</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>1109.0100</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>1148.2500</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>55744193</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>45440</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>1102.4400</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>1149.3900</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>1098.8300</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>1139.0100</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>65272789</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>45436</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>1044.4900</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>1064.7500</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>1030.0000</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>1064.6900</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>42949367</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>45435</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>1020.2800</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>1063.2000</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>1015.2000</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>1037.9900</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>83506528</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>954.5900</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>960.2000</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>932.4900</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>949.5000</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>54864799</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>45433</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>935.9900</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>954.0000</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>931.8000</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>953.8600</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>32894646</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>45432</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>937.5000</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>952.0000</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>934.4000</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>947.8000</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>31876446</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>45429</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>943.6900</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>947.4000</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>918.0600</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>924.7900</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>35969103</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>45428</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>949.1000</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>958.1899</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>941.0300</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>943.5900</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>32395182</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>45427</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>924.7200</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>948.6200</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>915.9900</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>946.3000</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>41773545</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>45426</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>895.9900</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>916.5100</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>889.3400</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>913.5600</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>29650708</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>45425</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>904.7800</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>909.9800</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>885.2900</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>903.9900</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>28968017</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>45422</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>903.0450</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>914.0100</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>892.2700</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>898.7800</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>33532541</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45421</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>905.2900</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>910.7200</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>882.3100</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>887.4700</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>37801268</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>45420</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>894.8250</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>911.9400</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>894.2000</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>904.1200</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>32572102</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>45419</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>910.9800</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>917.8099</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>890.1100</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>905.5400</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>43734161</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>45418</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>893.9000</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>922.2000</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>890.5500</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>921.4000</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>37620255</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>45415</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>877.8900</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>892.8100</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>870.4000</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>887.8900</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>39834072</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>45414</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>844.4900</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>862.3700</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>832.0000</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>858.1700</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>37789754</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>45413</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>850.7700</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>860.0000</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>812.5456</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>830.4100</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>55986317</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>45412</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>872.4000</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>888.1900</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>863.0000</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>864.0200</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>36370870</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>875.9500</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>879.9200</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>852.6600</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>877.5700</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>38897076</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="n">
+        <v>45408</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>838.1800</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>883.3093</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>833.8700</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>877.3500</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>55101078</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>45407</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>788.6801</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>833.2299</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>782.2300</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>826.3200</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>42464073</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n">
+        <v>45406</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>839.5000</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>840.8200</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>791.8300</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>796.7700</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>51220753</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="n">
+        <v>45405</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>807.6900</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>827.6900</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>802.6400</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>824.2300</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>43855937</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>45404</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>781.0400</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>800.7300</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>764.0000</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>795.1800</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>59634051</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>45401</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>831.5000</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>843.2400</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>756.0600</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>762.0000</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>87519800</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n">
+        <v>45400</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>849.7000</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>861.8999</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>824.0200</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>846.7100</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>44726034</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>45399</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>883.4000</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>887.7500</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>839.5000</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>840.3500</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>49539951</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>45398</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>864.3250</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>881.1800</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>860.6390</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>874.1500</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>37045302</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="n">
+        <v>45397</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>890.9800</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>906.1300</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>859.2901</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>860.0100</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>44307695</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="n">
+        <v>45394</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>896.9900</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>901.7499</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>875.3000</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>881.8600</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>42680479</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="n">
+        <v>45393</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>874.2000</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>907.3899</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>869.2600</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>906.1600</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>43163727</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>45392</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>839.2600</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>874.0000</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>837.0900</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>870.3900</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>43192853</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="n">
+        <v>45391</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>874.4200</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>876.3500</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>830.2200</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>853.5400</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>49977974</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>45390</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>887.0000</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>888.3000</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>867.3200</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>871.3300</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>27907532</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>45387</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>868.6600</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>884.8100</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>859.2600</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>880.0800</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>39772878</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>45386</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>904.0600</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>906.3399</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>858.8000</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>859.0500</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>42886990</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>45385</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>884.8400</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>903.7400</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>884.0000</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>889.6400</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>36759126</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>45384</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>884.4800</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>900.9400</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>876.2000</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>894.5200</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>43137935</t>
         </is>
       </c>
     </row>

</xml_diff>